<commit_message>
Update of cost tables
</commit_message>
<xml_diff>
--- a/ProjectMaker/.templates/REACH_stn_vii_TEMPLATE/REACH_stn_assessment_vii.xlsx
+++ b/ProjectMaker/.templates/REACH_stn_vii_TEMPLATE/REACH_stn_assessment_vii.xlsx
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="125">
   <si>
     <t>Reach:</t>
   </si>
@@ -568,16 +568,31 @@
   <si>
     <t>Net gain in AUA (ac/yr):</t>
   </si>
+  <si>
+    <t>FEES AND LICENSING</t>
+  </si>
+  <si>
+    <t>Markups (overhead, profit, insurance) and Engineering fees</t>
+  </si>
+  <si>
+    <t>Permitting</t>
+  </si>
+  <si>
+    <t>LCH (2012)
+Cramer (2012)
+Johnson (2019)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1046,7 +1061,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="7"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1462,27 +1477,75 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="13" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1491,51 +1554,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1545,6 +1563,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22" customBuiltin="1"/>
@@ -1909,16 +1930,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="143" t="s">
+      <c r="B1" s="161" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
     </row>
     <row r="2" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="75" t="s">
@@ -1936,15 +1957,15 @@
         <f>G60</f>
         <v>0</v>
       </c>
-      <c r="H2" s="144" t="s">
+      <c r="H2" s="162" t="s">
         <v>117</v>
       </c>
-      <c r="I2" s="146" t="str">
+      <c r="I2" s="163" t="str">
         <f>IF(NOT(OR(ISBLANK(G2), ISBLANK(G3))),G2/G3,"")</f>
         <v/>
       </c>
       <c r="J2" s="81"/>
-      <c r="K2" s="148" t="s">
+      <c r="K2" s="164" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1956,15 +1977,15 @@
         <v>100</v>
       </c>
       <c r="D3" s="80"/>
-      <c r="E3" s="150" t="s">
+      <c r="E3" s="166" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="151"/>
+      <c r="F3" s="146"/>
       <c r="G3" s="99"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="147"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="150"/>
       <c r="J3" s="81"/>
-      <c r="K3" s="149"/>
+      <c r="K3" s="165"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="82"/>
@@ -2013,7 +2034,7 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="2:11" s="139" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="141" t="s">
+      <c r="B7" s="160" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2039,7 +2060,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" s="139" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="142"/>
+      <c r="B8" s="157"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
@@ -2064,7 +2085,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" s="139" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="142"/>
+      <c r="B9" s="157"/>
       <c r="C9" s="61" t="s">
         <v>19</v>
       </c>
@@ -2085,13 +2106,13 @@
       </c>
     </row>
     <row r="10" spans="2:11" s="139" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="156" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="142"/>
-      <c r="D10" s="142"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="142"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="157"/>
+      <c r="E10" s="157"/>
+      <c r="F10" s="157"/>
       <c r="G10" s="111">
         <f>SUM(G7:G9)</f>
         <v>0</v>
@@ -2110,7 +2131,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="2:11" s="139" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="155" t="s">
+      <c r="B12" s="158" t="s">
         <v>112</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2138,7 +2159,7 @@
       </c>
     </row>
     <row r="13" spans="2:11" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="153"/>
+      <c r="B13" s="154"/>
       <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
@@ -2165,7 +2186,7 @@
       </c>
     </row>
     <row r="14" spans="2:11" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="153"/>
+      <c r="B14" s="154"/>
       <c r="C14" s="5" t="s">
         <v>30</v>
       </c>
@@ -2187,7 +2208,7 @@
       </c>
     </row>
     <row r="15" spans="2:11" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="153"/>
+      <c r="B15" s="154"/>
       <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
@@ -2209,7 +2230,7 @@
       </c>
     </row>
     <row r="16" spans="2:11" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="153"/>
+      <c r="B16" s="154"/>
       <c r="C16" s="64" t="s">
         <v>34</v>
       </c>
@@ -2233,13 +2254,13 @@
       </c>
     </row>
     <row r="17" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="156" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="153"/>
-      <c r="D17" s="153"/>
-      <c r="E17" s="153"/>
-      <c r="F17" s="153"/>
+      <c r="C17" s="154"/>
+      <c r="D17" s="154"/>
+      <c r="E17" s="154"/>
+      <c r="F17" s="154"/>
       <c r="G17" s="111">
         <f>SUM(G12:G16)</f>
         <v>0</v>
@@ -2258,7 +2279,7 @@
       <c r="I18" s="16"/>
     </row>
     <row r="19" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="155" t="s">
+      <c r="B19" s="158" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -2282,7 +2303,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="156"/>
+      <c r="B20" s="143"/>
       <c r="C20" s="9" t="s">
         <v>40</v>
       </c>
@@ -2304,7 +2325,7 @@
       </c>
     </row>
     <row r="21" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="153"/>
+      <c r="B21" s="154"/>
       <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
@@ -2327,7 +2348,7 @@
       </c>
     </row>
     <row r="22" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="153"/>
+      <c r="B22" s="154"/>
       <c r="C22" s="5" t="s">
         <v>45</v>
       </c>
@@ -2350,7 +2371,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="153"/>
+      <c r="B23" s="154"/>
       <c r="C23" s="5" t="s">
         <v>46</v>
       </c>
@@ -2376,7 +2397,7 @@
       </c>
     </row>
     <row r="24" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="153"/>
+      <c r="B24" s="154"/>
       <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
@@ -2402,7 +2423,7 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="156"/>
+      <c r="B25" s="143"/>
       <c r="C25" s="22" t="s">
         <v>49</v>
       </c>
@@ -2426,7 +2447,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="156"/>
+      <c r="B26" s="143"/>
       <c r="C26" s="67" t="s">
         <v>51</v>
       </c>
@@ -2450,13 +2471,13 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="154" t="s">
+      <c r="B27" s="156" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="156"/>
-      <c r="D27" s="157"/>
-      <c r="E27" s="158"/>
-      <c r="F27" s="151"/>
+      <c r="C27" s="143"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="146"/>
       <c r="G27" s="111">
         <f>SUM(G19:G26)</f>
         <v>0</v>
@@ -2500,7 +2521,7 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="156"/>
+      <c r="B30" s="143"/>
       <c r="C30" s="9" t="s">
         <v>56</v>
       </c>
@@ -2523,7 +2544,7 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="156"/>
+      <c r="B31" s="143"/>
       <c r="C31" s="9" t="s">
         <v>58</v>
       </c>
@@ -2547,7 +2568,7 @@
       </c>
     </row>
     <row r="32" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="153"/>
+      <c r="B32" s="154"/>
       <c r="C32" s="5" t="s">
         <v>60</v>
       </c>
@@ -2574,7 +2595,7 @@
       </c>
     </row>
     <row r="33" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="153"/>
+      <c r="B33" s="154"/>
       <c r="C33" s="64" t="s">
         <v>62</v>
       </c>
@@ -2601,13 +2622,13 @@
       </c>
     </row>
     <row r="34" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="154" t="s">
+      <c r="B34" s="156" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="156"/>
-      <c r="D34" s="157"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="151"/>
+      <c r="C34" s="143"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="145"/>
+      <c r="F34" s="146"/>
       <c r="G34" s="111">
         <f>SUM(G29:G33)</f>
         <v>0</v>
@@ -2626,7 +2647,7 @@
       <c r="I35" s="27"/>
     </row>
     <row r="36" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="155" t="s">
+      <c r="B36" s="158" t="s">
         <v>65</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -2649,7 +2670,7 @@
       </c>
     </row>
     <row r="37" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="153"/>
+      <c r="B37" s="154"/>
       <c r="C37" s="64" t="s">
         <v>68</v>
       </c>
@@ -2671,13 +2692,13 @@
       </c>
     </row>
     <row r="38" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="154" t="s">
+      <c r="B38" s="156" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="153"/>
-      <c r="D38" s="153"/>
-      <c r="E38" s="153"/>
-      <c r="F38" s="153"/>
+      <c r="C38" s="154"/>
+      <c r="D38" s="154"/>
+      <c r="E38" s="154"/>
+      <c r="F38" s="154"/>
       <c r="G38" s="111">
         <f>SUM(G36:G37)</f>
         <v>0</v>
@@ -2696,7 +2717,7 @@
       <c r="I39" s="16"/>
     </row>
     <row r="40" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="155" t="s">
+      <c r="B40" s="158" t="s">
         <v>70</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -2719,7 +2740,7 @@
       </c>
     </row>
     <row r="41" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="153"/>
+      <c r="B41" s="154"/>
       <c r="C41" s="5" t="s">
         <v>72</v>
       </c>
@@ -2740,7 +2761,7 @@
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="156"/>
+      <c r="B42" s="143"/>
       <c r="C42" s="9" t="s">
         <v>74</v>
       </c>
@@ -2763,7 +2784,7 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="156"/>
+      <c r="B43" s="143"/>
       <c r="C43" s="9" t="s">
         <v>76</v>
       </c>
@@ -2784,7 +2805,7 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="156"/>
+      <c r="B44" s="143"/>
       <c r="C44" s="9" t="s">
         <v>77</v>
       </c>
@@ -2805,7 +2826,7 @@
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="156"/>
+      <c r="B45" s="143"/>
       <c r="C45" s="9" t="s">
         <v>78</v>
       </c>
@@ -2826,7 +2847,7 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="156"/>
+      <c r="B46" s="143"/>
       <c r="C46" s="9" t="s">
         <v>79</v>
       </c>
@@ -2847,7 +2868,7 @@
       </c>
     </row>
     <row r="47" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="153"/>
+      <c r="B47" s="154"/>
       <c r="C47" s="64" t="s">
         <v>102</v>
       </c>
@@ -2869,13 +2890,13 @@
       </c>
     </row>
     <row r="48" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="154" t="s">
+      <c r="B48" s="156" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="153"/>
-      <c r="D48" s="153"/>
-      <c r="E48" s="153"/>
-      <c r="F48" s="153"/>
+      <c r="C48" s="154"/>
+      <c r="D48" s="154"/>
+      <c r="E48" s="154"/>
+      <c r="F48" s="154"/>
       <c r="G48" s="111">
         <f>SUM(G40:G47)</f>
         <v>0</v>
@@ -2894,13 +2915,13 @@
       <c r="I49" s="38"/>
     </row>
     <row r="50" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="152" t="s">
+      <c r="B50" s="155" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="153"/>
-      <c r="D50" s="153"/>
-      <c r="E50" s="153"/>
-      <c r="F50" s="153"/>
+      <c r="C50" s="154"/>
+      <c r="D50" s="154"/>
+      <c r="E50" s="154"/>
+      <c r="F50" s="154"/>
       <c r="G50" s="122">
         <f>SUM(G48,G38,G34,G27,G17,G10)</f>
         <v>0</v>
@@ -2909,16 +2930,16 @@
       <c r="I50" s="38"/>
     </row>
     <row r="52" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="161" t="s">
+      <c r="B52" s="147" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="156"/>
-      <c r="D52" s="157"/>
-      <c r="E52" s="158"/>
-      <c r="F52" s="151"/>
-      <c r="G52" s="162"/>
-      <c r="H52" s="145"/>
-      <c r="I52" s="147"/>
+      <c r="C52" s="143"/>
+      <c r="D52" s="144"/>
+      <c r="E52" s="145"/>
+      <c r="F52" s="146"/>
+      <c r="G52" s="148"/>
+      <c r="H52" s="149"/>
+      <c r="I52" s="150"/>
     </row>
     <row r="53" spans="2:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="32"/>
@@ -2931,10 +2952,10 @@
       <c r="I53" s="32"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="163" t="s">
+      <c r="B54" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="156"/>
+      <c r="C54" s="143"/>
       <c r="D54" s="31"/>
       <c r="E54" s="28"/>
       <c r="F54" s="55"/>
@@ -2943,10 +2964,10 @@
       <c r="I54" s="30"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="164" t="s">
+      <c r="B55" s="152" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="156"/>
+      <c r="C55" s="143"/>
       <c r="D55" s="34">
         <v>0.1</v>
       </c>
@@ -2965,10 +2986,10 @@
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B56" s="164" t="s">
+      <c r="B56" s="152" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="156"/>
+      <c r="C56" s="143"/>
       <c r="D56" s="35">
         <v>0.1</v>
       </c>
@@ -2987,10 +3008,10 @@
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B57" s="163" t="s">
+      <c r="B57" s="151" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="156"/>
+      <c r="C57" s="143"/>
       <c r="D57" s="36"/>
       <c r="E57" s="28"/>
       <c r="F57" s="55"/>
@@ -2999,10 +3020,10 @@
       <c r="I57" s="30"/>
     </row>
     <row r="58" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="165" t="s">
+      <c r="B58" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="C58" s="153"/>
+      <c r="C58" s="154"/>
       <c r="D58" s="58">
         <f>AVERAGE(0.1,0.2)</f>
         <v>0.15000000000000002</v>
@@ -3023,13 +3044,13 @@
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B60" s="160" t="s">
+      <c r="B60" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="156"/>
-      <c r="D60" s="157"/>
-      <c r="E60" s="158"/>
-      <c r="F60" s="151"/>
+      <c r="C60" s="143"/>
+      <c r="D60" s="144"/>
+      <c r="E60" s="145"/>
+      <c r="F60" s="146"/>
       <c r="G60" s="125">
         <f>G58+G56+G55+G50</f>
         <v>0</v>
@@ -3039,13 +3060,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="B50:F50"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B12:B16"/>
@@ -3058,12 +3078,13 @@
     <mergeCell ref="B38:F38"/>
     <mergeCell ref="B40:B47"/>
     <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:F11 B17:F18 B27:F28 B34:F35 B38:F39 B48:F49">
     <cfRule type="expression" dxfId="9" priority="5">
@@ -3094,10 +3115,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K60"/>
+  <dimension ref="B1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:F17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3117,16 +3138,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="143" t="s">
+      <c r="B1" s="161" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="161"/>
+      <c r="I1" s="161"/>
     </row>
     <row r="2" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="75" t="s">
@@ -3141,18 +3162,18 @@
         <v>1</v>
       </c>
       <c r="G2" s="98">
-        <f>G60</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="144" t="s">
+        <f>G61</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="162" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="146" t="str">
+      <c r="I2" s="163" t="str">
         <f>IF(NOT(OR(ISBLANK(G2), ISBLANK(G3))),G2/G3,"")</f>
         <v/>
       </c>
       <c r="J2" s="81"/>
-      <c r="K2" s="148" t="s">
+      <c r="K2" s="164" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3164,15 +3185,15 @@
         <v>100</v>
       </c>
       <c r="D3" s="80"/>
-      <c r="E3" s="150" t="s">
+      <c r="E3" s="166" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="151"/>
+      <c r="F3" s="146"/>
       <c r="G3" s="99"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="147"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="150"/>
       <c r="J3" s="81"/>
-      <c r="K3" s="149"/>
+      <c r="K3" s="165"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="82"/>
@@ -3221,7 +3242,7 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="141" t="s">
+      <c r="B7" s="160" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -3247,13 +3268,12 @@
       </c>
     </row>
     <row r="8" spans="2:11" s="91" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="142"/>
+      <c r="B8" s="157"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="107">
-        <f>AVERAGE(10, 6*1.65, 9*1.296)</f>
-        <v>10.521333333333333</v>
+        <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
@@ -3262,7 +3282,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="108">
-        <f>D8/2*MIN(terraforming_volumes!C5,terraforming_volumes!C6)+'costs (U.S. Cust.)'!D8*(MAX(terraforming_volumes!C5,terraforming_volumes!C6)-MIN(terraforming_volumes!C5,terraforming_volumes!C6))</f>
+        <f>D8*MAX(terraforming_volumes!C5,terraforming_volumes!C6)</f>
         <v>0</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -3273,7 +3293,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="142"/>
+      <c r="B9" s="157"/>
       <c r="C9" s="61" t="s">
         <v>19</v>
       </c>
@@ -3294,13 +3314,13 @@
       </c>
     </row>
     <row r="10" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="156" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="142"/>
-      <c r="D10" s="142"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="142"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="157"/>
+      <c r="E10" s="157"/>
+      <c r="F10" s="157"/>
       <c r="G10" s="111">
         <f>SUM(G7:G9)</f>
         <v>0</v>
@@ -3319,7 +3339,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="155" t="s">
+      <c r="B12" s="158" t="s">
         <v>112</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -3347,7 +3367,7 @@
       </c>
     </row>
     <row r="13" spans="2:11" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="153"/>
+      <c r="B13" s="154"/>
       <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
@@ -3374,7 +3394,7 @@
       </c>
     </row>
     <row r="14" spans="2:11" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="153"/>
+      <c r="B14" s="154"/>
       <c r="C14" s="5" t="s">
         <v>30</v>
       </c>
@@ -3396,7 +3416,7 @@
       </c>
     </row>
     <row r="15" spans="2:11" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="153"/>
+      <c r="B15" s="154"/>
       <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
@@ -3418,13 +3438,12 @@
       </c>
     </row>
     <row r="16" spans="2:11" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="153"/>
+      <c r="B16" s="154"/>
       <c r="C16" s="64" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="114">
-        <f>AVERAGE(120,230,10,160)</f>
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E16" s="65" t="s">
         <v>35</v>
@@ -3443,13 +3462,13 @@
       </c>
     </row>
     <row r="17" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="156" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="153"/>
-      <c r="D17" s="153"/>
-      <c r="E17" s="153"/>
-      <c r="F17" s="153"/>
+      <c r="C17" s="154"/>
+      <c r="D17" s="154"/>
+      <c r="E17" s="154"/>
+      <c r="F17" s="154"/>
       <c r="G17" s="111">
         <f>SUM(G12:G16)</f>
         <v>0</v>
@@ -3468,7 +3487,7 @@
       <c r="I18" s="16"/>
     </row>
     <row r="19" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="155" t="s">
+      <c r="B19" s="158" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -3492,7 +3511,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="156"/>
+      <c r="B20" s="143"/>
       <c r="C20" s="9" t="s">
         <v>40</v>
       </c>
@@ -3514,7 +3533,7 @@
       </c>
     </row>
     <row r="21" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="153"/>
+      <c r="B21" s="154"/>
       <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
@@ -3538,7 +3557,7 @@
       </c>
     </row>
     <row r="22" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="153"/>
+      <c r="B22" s="154"/>
       <c r="C22" s="5" t="s">
         <v>45</v>
       </c>
@@ -3562,7 +3581,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="153"/>
+      <c r="B23" s="154"/>
       <c r="C23" s="5" t="s">
         <v>46</v>
       </c>
@@ -3588,7 +3607,7 @@
       </c>
     </row>
     <row r="24" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="153"/>
+      <c r="B24" s="154"/>
       <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
@@ -3614,7 +3633,7 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="156"/>
+      <c r="B25" s="143"/>
       <c r="C25" s="22" t="s">
         <v>49</v>
       </c>
@@ -3639,7 +3658,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="156"/>
+      <c r="B26" s="143"/>
       <c r="C26" s="67" t="s">
         <v>51</v>
       </c>
@@ -3664,13 +3683,13 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="154" t="s">
+      <c r="B27" s="156" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="156"/>
-      <c r="D27" s="157"/>
-      <c r="E27" s="158"/>
-      <c r="F27" s="151"/>
+      <c r="C27" s="143"/>
+      <c r="D27" s="144"/>
+      <c r="E27" s="145"/>
+      <c r="F27" s="146"/>
       <c r="G27" s="111">
         <f>SUM(G19:G26)</f>
         <v>0</v>
@@ -3715,7 +3734,7 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="156"/>
+      <c r="B30" s="143"/>
       <c r="C30" s="9" t="s">
         <v>56</v>
       </c>
@@ -3739,7 +3758,7 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="156"/>
+      <c r="B31" s="143"/>
       <c r="C31" s="9" t="s">
         <v>58</v>
       </c>
@@ -3763,7 +3782,7 @@
       </c>
     </row>
     <row r="32" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="153"/>
+      <c r="B32" s="154"/>
       <c r="C32" s="5" t="s">
         <v>60</v>
       </c>
@@ -3790,7 +3809,7 @@
       </c>
     </row>
     <row r="33" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="153"/>
+      <c r="B33" s="154"/>
       <c r="C33" s="64" t="s">
         <v>62</v>
       </c>
@@ -3817,13 +3836,13 @@
       </c>
     </row>
     <row r="34" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="154" t="s">
+      <c r="B34" s="156" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="156"/>
-      <c r="D34" s="157"/>
-      <c r="E34" s="158"/>
-      <c r="F34" s="151"/>
+      <c r="C34" s="143"/>
+      <c r="D34" s="144"/>
+      <c r="E34" s="145"/>
+      <c r="F34" s="146"/>
       <c r="G34" s="111">
         <f>SUM(G29:G33)</f>
         <v>0</v>
@@ -3842,7 +3861,7 @@
       <c r="I35" s="27"/>
     </row>
     <row r="36" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="155" t="s">
+      <c r="B36" s="158" t="s">
         <v>65</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -3866,7 +3885,7 @@
       </c>
     </row>
     <row r="37" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="153"/>
+      <c r="B37" s="154"/>
       <c r="C37" s="64" t="s">
         <v>68</v>
       </c>
@@ -3888,13 +3907,13 @@
       </c>
     </row>
     <row r="38" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="154" t="s">
+      <c r="B38" s="156" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="153"/>
-      <c r="D38" s="153"/>
-      <c r="E38" s="153"/>
-      <c r="F38" s="153"/>
+      <c r="C38" s="154"/>
+      <c r="D38" s="154"/>
+      <c r="E38" s="154"/>
+      <c r="F38" s="154"/>
       <c r="G38" s="111">
         <f>SUM(G36:G37)</f>
         <v>0</v>
@@ -3913,7 +3932,7 @@
       <c r="I39" s="16"/>
     </row>
     <row r="40" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="155" t="s">
+      <c r="B40" s="158" t="s">
         <v>70</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -3936,7 +3955,7 @@
       </c>
     </row>
     <row r="41" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="153"/>
+      <c r="B41" s="154"/>
       <c r="C41" s="5" t="s">
         <v>72</v>
       </c>
@@ -3958,12 +3977,12 @@
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="156"/>
+      <c r="B42" s="143"/>
       <c r="C42" s="9" t="s">
         <v>74</v>
       </c>
       <c r="D42" s="116">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>24</v>
@@ -3981,7 +4000,7 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="156"/>
+      <c r="B43" s="143"/>
       <c r="C43" s="9" t="s">
         <v>76</v>
       </c>
@@ -4002,7 +4021,7 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="156"/>
+      <c r="B44" s="143"/>
       <c r="C44" s="9" t="s">
         <v>77</v>
       </c>
@@ -4023,7 +4042,7 @@
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="156"/>
+      <c r="B45" s="143"/>
       <c r="C45" s="9" t="s">
         <v>78</v>
       </c>
@@ -4044,7 +4063,7 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="156"/>
+      <c r="B46" s="143"/>
       <c r="C46" s="9" t="s">
         <v>79</v>
       </c>
@@ -4065,7 +4084,7 @@
       </c>
     </row>
     <row r="47" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="153"/>
+      <c r="B47" s="154"/>
       <c r="C47" s="64" t="s">
         <v>102</v>
       </c>
@@ -4087,13 +4106,13 @@
       </c>
     </row>
     <row r="48" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="154" t="s">
+      <c r="B48" s="156" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="153"/>
-      <c r="D48" s="153"/>
-      <c r="E48" s="153"/>
-      <c r="F48" s="153"/>
+      <c r="C48" s="154"/>
+      <c r="D48" s="154"/>
+      <c r="E48" s="154"/>
+      <c r="F48" s="154"/>
       <c r="G48" s="111">
         <f>SUM(G40:G47)</f>
         <v>0</v>
@@ -4112,13 +4131,13 @@
       <c r="I49" s="38"/>
     </row>
     <row r="50" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="152" t="s">
+      <c r="B50" s="155" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="153"/>
-      <c r="D50" s="153"/>
-      <c r="E50" s="153"/>
-      <c r="F50" s="153"/>
+      <c r="C50" s="154"/>
+      <c r="D50" s="154"/>
+      <c r="E50" s="154"/>
+      <c r="F50" s="154"/>
       <c r="G50" s="122">
         <f>SUM(G48,G38,G34,G27,G17,G10)</f>
         <v>0</v>
@@ -4127,16 +4146,16 @@
       <c r="I50" s="38"/>
     </row>
     <row r="52" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="161" t="s">
+      <c r="B52" s="147" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="156"/>
-      <c r="D52" s="157"/>
-      <c r="E52" s="158"/>
-      <c r="F52" s="151"/>
-      <c r="G52" s="162"/>
-      <c r="H52" s="145"/>
-      <c r="I52" s="147"/>
+      <c r="C52" s="143"/>
+      <c r="D52" s="144"/>
+      <c r="E52" s="145"/>
+      <c r="F52" s="146"/>
+      <c r="G52" s="148"/>
+      <c r="H52" s="149"/>
+      <c r="I52" s="150"/>
     </row>
     <row r="53" spans="2:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="32"/>
@@ -4149,10 +4168,10 @@
       <c r="I53" s="32"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="163" t="s">
+      <c r="B54" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="156"/>
+      <c r="C54" s="143"/>
       <c r="D54" s="31"/>
       <c r="E54" s="28"/>
       <c r="F54" s="55"/>
@@ -4161,10 +4180,10 @@
       <c r="I54" s="30"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="164" t="s">
+      <c r="B55" s="152" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="156"/>
+      <c r="C55" s="143"/>
       <c r="D55" s="34">
         <v>0.1</v>
       </c>
@@ -4183,10 +4202,10 @@
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B56" s="164" t="s">
+      <c r="B56" s="152" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="156"/>
+      <c r="C56" s="143"/>
       <c r="D56" s="35">
         <v>0.1</v>
       </c>
@@ -4205,10 +4224,10 @@
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B57" s="163" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="156"/>
+      <c r="B57" s="151" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="143"/>
       <c r="D57" s="36"/>
       <c r="E57" s="28"/>
       <c r="F57" s="55"/>
@@ -4216,14 +4235,13 @@
       <c r="H57" s="29"/>
       <c r="I57" s="30"/>
     </row>
-    <row r="58" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="165" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="153"/>
-      <c r="D58" s="58">
-        <f>AVERAGE(0.1,0.2)</f>
-        <v>0.15000000000000002</v>
+    <row r="58" spans="2:9" s="90" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="153" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="154"/>
+      <c r="D58" s="171">
+        <v>0.16500000000000001</v>
       </c>
       <c r="E58" s="59" t="s">
         <v>86</v>
@@ -4237,26 +4255,57 @@
       </c>
       <c r="H58" s="37"/>
       <c r="I58" s="38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B60" s="160" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" s="141" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="153" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="154"/>
+      <c r="D59" s="58">
+        <v>0.35</v>
+      </c>
+      <c r="E59" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="F59" s="60">
+        <v>1</v>
+      </c>
+      <c r="G59" s="124">
+        <f>G50*D59</f>
+        <v>0</v>
+      </c>
+      <c r="H59" s="37"/>
+      <c r="I59" s="38"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B61" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="156"/>
-      <c r="D60" s="157"/>
-      <c r="E60" s="158"/>
-      <c r="F60" s="151"/>
-      <c r="G60" s="125">
-        <f>G58+G56+G55+G50</f>
-        <v>0</v>
-      </c>
-      <c r="H60" s="92"/>
-      <c r="I60" s="92"/>
+      <c r="C61" s="143"/>
+      <c r="D61" s="144"/>
+      <c r="E61" s="145"/>
+      <c r="F61" s="146"/>
+      <c r="G61" s="125">
+        <f>G58+G56+G55+G50+G59</f>
+        <v>0</v>
+      </c>
+      <c r="H61" s="92"/>
+      <c r="I61" s="92"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B59:C59"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="B48:F48"/>
@@ -4273,15 +4322,6 @@
     <mergeCell ref="B29:B33"/>
     <mergeCell ref="B36:B37"/>
     <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B55:C55"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:F11 B17:F18 B27:F28 B34:F35 B38:F39 B48:F49">
     <cfRule type="expression" dxfId="4" priority="5">
@@ -4385,27 +4425,27 @@
       <c r="B2" s="94" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="167" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
-      <c r="I2" s="167"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="168"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="168" t="s">
+      <c r="B3" s="169" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
+      <c r="F3" s="170"/>
+      <c r="G3" s="170"/>
+      <c r="H3" s="170"/>
+      <c r="I3" s="170"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="95"/>

</xml_diff>

<commit_message>
Add user-defined season limits to HabitatEvaluation
</commit_message>
<xml_diff>
--- a/ProjectMaker/.templates/REACH_stn_vii_TEMPLATE/REACH_stn_assessment_vii.xlsx
+++ b/ProjectMaker/.templates/REACH_stn_vii_TEMPLATE/REACH_stn_assessment_vii.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\RA_development\ProjectMaker\.templates\REACH_stn_vii_TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\RiverArchitect\ProjectMaker\.templates\REACH_stn_vii_TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -545,10 +545,6 @@
     <t>Generated  with the RiverArchitect's ModifyTerrain module</t>
   </si>
   <si>
-    <t>Project return
-(US $ per m² net gain in AUA)</t>
-  </si>
-  <si>
     <t>Net gain in AUA (m²/yr):</t>
   </si>
   <si>
@@ -560,9 +556,6 @@
   </si>
   <si>
     <t>FEES AND LICENSING</t>
-  </si>
-  <si>
-    <t>Markups (overhead, profit, insurance) and Engineering fees</t>
   </si>
   <si>
     <t>Permitting</t>
@@ -571,18 +564,27 @@
     <t>LCH (2012)
 Cramer (2012)
 Johnson (2019)</t>
+  </si>
+  <si>
+    <t>Project return
+(EUR per m² net gain in AUA)</t>
+  </si>
+  <si>
+    <t>Markups (overhead, profit, insurance) and 
+Engineering fees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="_([$EUR]\ * #,##0.00_);_([$EUR]\ * \(#,##0.00\);_([$EUR]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1051,7 +1053,7 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="7"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1476,27 +1478,72 @@
     <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="13" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1505,51 +1552,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1559,6 +1561,69 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22" customBuiltin="1"/>
@@ -1902,15 +1967,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="132" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" style="132" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="133" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="133" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="134" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="135" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" style="136" customWidth="1"/>
@@ -1923,16 +1988,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="163" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
     </row>
     <row r="2" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="75" t="s">
@@ -1946,19 +2011,19 @@
       <c r="F2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="98">
+      <c r="G2" s="192">
         <f>G61</f>
         <v>0</v>
       </c>
-      <c r="H2" s="147" t="s">
-        <v>114</v>
-      </c>
-      <c r="I2" s="149" t="str">
+      <c r="H2" s="164" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="165" t="str">
         <f>IF(NOT(OR(ISBLANK(G2), ISBLANK(G3))),G2/G3,"")</f>
         <v/>
       </c>
       <c r="J2" s="81"/>
-      <c r="K2" s="151" t="s">
+      <c r="K2" s="166" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1970,15 +2035,15 @@
         <v>97</v>
       </c>
       <c r="D3" s="80"/>
-      <c r="E3" s="153" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" s="154"/>
+      <c r="E3" s="168" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="148"/>
       <c r="G3" s="99"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="150"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="152"/>
       <c r="J3" s="81"/>
-      <c r="K3" s="152"/>
+      <c r="K3" s="167"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="82"/>
@@ -2027,13 +2092,13 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="2:11" s="139" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="144" t="s">
+      <c r="B7" s="162" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="105">
+      <c r="D7" s="173">
         <v>5.4399999999999997E-2</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -2043,7 +2108,7 @@
         <f>from_geodata!C4</f>
         <v>0</v>
       </c>
-      <c r="G7" s="106">
+      <c r="G7" s="173">
         <f>F7*D7</f>
         <v>0</v>
       </c>
@@ -2053,12 +2118,12 @@
       </c>
     </row>
     <row r="8" spans="2:11" s="139" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="145"/>
+      <c r="B8" s="159"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="107">
-        <v>25</v>
+      <c r="D8" s="174">
+        <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>106</v>
@@ -2066,7 +2131,7 @@
       <c r="F8" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="108">
+      <c r="G8" s="176">
         <f>D8/2*MIN(terraforming_volumes!C5,terraforming_volumes!C6)+'costs (SI metric)'!D8*(MAX(terraforming_volumes!C5,terraforming_volumes!C6)-MIN(terraforming_volumes!C5,terraforming_volumes!C6))</f>
         <v>0</v>
       </c>
@@ -2078,18 +2143,18 @@
       </c>
     </row>
     <row r="9" spans="2:11" s="139" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="145"/>
+      <c r="B9" s="159"/>
       <c r="C9" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="109">
+      <c r="D9" s="175">
         <v>1200</v>
       </c>
       <c r="E9" s="62" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="63"/>
-      <c r="G9" s="110">
+      <c r="G9" s="181">
         <f>F9*D9</f>
         <v>0</v>
       </c>
@@ -2099,14 +2164,14 @@
       </c>
     </row>
     <row r="10" spans="2:11" s="139" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="158" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="145"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="145"/>
-      <c r="G10" s="111">
+      <c r="C10" s="159"/>
+      <c r="D10" s="159"/>
+      <c r="E10" s="159"/>
+      <c r="F10" s="159"/>
+      <c r="G10" s="182">
         <f>SUM(G7:G9)</f>
         <v>0</v>
       </c>
@@ -2119,18 +2184,18 @@
       <c r="D11" s="69"/>
       <c r="E11" s="69"/>
       <c r="F11" s="70"/>
-      <c r="G11" s="112"/>
+      <c r="G11" s="183"/>
       <c r="H11" s="13"/>
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="2:11" s="139" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="158" t="s">
+      <c r="B12" s="160" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="105">
+      <c r="D12" s="173">
         <v>80</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -2140,7 +2205,7 @@
         <f>F13*log_length</f>
         <v>0</v>
       </c>
-      <c r="G12" s="106">
+      <c r="G12" s="173">
         <f>F12*D12</f>
         <v>0</v>
       </c>
@@ -2156,7 +2221,7 @@
       <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="113">
+      <c r="D13" s="176">
         <f>AVERAGE(600,1000, 300, 1200)</f>
         <v>775</v>
       </c>
@@ -2167,7 +2232,7 @@
         <f>from_geodata!C15/log_length^2</f>
         <v>0</v>
       </c>
-      <c r="G13" s="108">
+      <c r="G13" s="176">
         <f>F13*D13</f>
         <v>0</v>
       </c>
@@ -2183,7 +2248,7 @@
       <c r="C14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="113">
+      <c r="D14" s="176">
         <f>(1.65*15+75)/2</f>
         <v>49.875</v>
       </c>
@@ -2191,7 +2256,7 @@
         <v>31</v>
       </c>
       <c r="F14" s="52"/>
-      <c r="G14" s="108">
+      <c r="G14" s="176">
         <f>F14*D14</f>
         <v>0</v>
       </c>
@@ -2205,7 +2270,7 @@
       <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="113">
+      <c r="D15" s="176">
         <f>AVERAGE(5000,20000, 30000, 100000)</f>
         <v>38750</v>
       </c>
@@ -2213,7 +2278,7 @@
         <v>20</v>
       </c>
       <c r="F15" s="52"/>
-      <c r="G15" s="108">
+      <c r="G15" s="176">
         <f>F15*D15</f>
         <v>0</v>
       </c>
@@ -2227,7 +2292,7 @@
       <c r="C16" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="114">
+      <c r="D16" s="177">
         <v>150</v>
       </c>
       <c r="E16" s="65" t="s">
@@ -2237,7 +2302,7 @@
         <f>from_geodata!C13</f>
         <v>0</v>
       </c>
-      <c r="G16" s="115">
+      <c r="G16" s="184">
         <f>F16*D16</f>
         <v>0</v>
       </c>
@@ -2247,14 +2312,14 @@
       </c>
     </row>
     <row r="17" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="157" t="s">
+      <c r="B17" s="158" t="s">
         <v>110</v>
       </c>
       <c r="C17" s="156"/>
       <c r="D17" s="156"/>
       <c r="E17" s="156"/>
       <c r="F17" s="156"/>
-      <c r="G17" s="111">
+      <c r="G17" s="182">
         <f>SUM(G12:G16)</f>
         <v>0</v>
       </c>
@@ -2267,18 +2332,18 @@
       <c r="D18" s="69"/>
       <c r="E18" s="69"/>
       <c r="F18" s="70"/>
-      <c r="G18" s="112"/>
+      <c r="G18" s="183"/>
       <c r="H18" s="15"/>
       <c r="I18" s="16"/>
     </row>
     <row r="19" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="158" t="s">
+      <c r="B19" s="160" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="107">
+      <c r="D19" s="174">
         <f>AVERAGE(120, 300)</f>
         <v>210</v>
       </c>
@@ -2286,7 +2351,7 @@
         <v>20</v>
       </c>
       <c r="F19" s="52"/>
-      <c r="G19" s="108">
+      <c r="G19" s="176">
         <f t="shared" ref="G19:G26" si="0">F19*D19</f>
         <v>0</v>
       </c>
@@ -2296,11 +2361,11 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="159"/>
+      <c r="B20" s="145"/>
       <c r="C20" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="116">
+      <c r="D20" s="178">
         <f>20*1.65</f>
         <v>33</v>
       </c>
@@ -2308,7 +2373,7 @@
         <v>41</v>
       </c>
       <c r="F20" s="53"/>
-      <c r="G20" s="117">
+      <c r="G20" s="185">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2322,14 +2387,14 @@
       <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="107">
+      <c r="D21" s="174">
         <v>18</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>105</v>
       </c>
       <c r="F21" s="52"/>
-      <c r="G21" s="108">
+      <c r="G21" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2345,14 +2410,14 @@
       <c r="C22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="107">
+      <c r="D22" s="174">
         <v>18</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>105</v>
       </c>
       <c r="F22" s="52"/>
-      <c r="G22" s="108">
+      <c r="G22" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2368,7 +2433,7 @@
       <c r="C23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="107">
+      <c r="D23" s="174">
         <v>10</v>
       </c>
       <c r="E23" s="6" t="s">
@@ -2378,7 +2443,7 @@
         <f>from_geodata!C8</f>
         <v>0</v>
       </c>
-      <c r="G23" s="108">
+      <c r="G23" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2394,7 +2459,7 @@
       <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="107">
+      <c r="D24" s="174">
         <v>10</v>
       </c>
       <c r="E24" s="6" t="s">
@@ -2404,7 +2469,7 @@
         <f>from_geodata!C7</f>
         <v>0</v>
       </c>
-      <c r="G24" s="108">
+      <c r="G24" s="176">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2416,11 +2481,11 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="159"/>
+      <c r="B25" s="145"/>
       <c r="C25" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="118">
+      <c r="D25" s="179">
         <v>10</v>
       </c>
       <c r="E25" s="6" t="s">
@@ -2430,7 +2495,7 @@
         <f>from_geodata!C5</f>
         <v>0</v>
       </c>
-      <c r="G25" s="117">
+      <c r="G25" s="185">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2440,11 +2505,11 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="159"/>
+      <c r="B26" s="145"/>
       <c r="C26" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="119">
+      <c r="D26" s="180">
         <v>10</v>
       </c>
       <c r="E26" s="68" t="s">
@@ -2454,7 +2519,7 @@
         <f>from_geodata!C6</f>
         <v>0</v>
       </c>
-      <c r="G26" s="120">
+      <c r="G26" s="186">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2464,14 +2529,14 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="157" t="s">
+      <c r="B27" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="159"/>
-      <c r="D27" s="160"/>
-      <c r="E27" s="161"/>
-      <c r="F27" s="154"/>
-      <c r="G27" s="111">
+      <c r="C27" s="145"/>
+      <c r="D27" s="146"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="148"/>
+      <c r="G27" s="182">
         <f>SUM(G19:G26)</f>
         <v>0</v>
       </c>
@@ -2484,25 +2549,25 @@
       <c r="D28" s="69"/>
       <c r="E28" s="69"/>
       <c r="F28" s="70"/>
-      <c r="G28" s="112"/>
+      <c r="G28" s="183"/>
       <c r="H28" s="26"/>
       <c r="I28" s="27"/>
     </row>
     <row r="29" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="162" t="s">
+      <c r="B29" s="161" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="116">
+      <c r="D29" s="178">
         <v>75</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>105</v>
       </c>
       <c r="F29" s="53"/>
-      <c r="G29" s="117">
+      <c r="G29" s="185">
         <f>F29*D29</f>
         <v>0</v>
       </c>
@@ -2514,18 +2579,18 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="159"/>
+      <c r="B30" s="145"/>
       <c r="C30" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="116">
+      <c r="D30" s="178">
         <v>35</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>107</v>
       </c>
       <c r="F30" s="53"/>
-      <c r="G30" s="117">
+      <c r="G30" s="185">
         <f>F30*D30</f>
         <v>0</v>
       </c>
@@ -2537,11 +2602,11 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="159"/>
+      <c r="B31" s="145"/>
       <c r="C31" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="116">
+      <c r="D31" s="178">
         <f>(2+10)/2</f>
         <v>6</v>
       </c>
@@ -2549,7 +2614,7 @@
         <v>105</v>
       </c>
       <c r="F31" s="53"/>
-      <c r="G31" s="117">
+      <c r="G31" s="185">
         <f>F31*D31</f>
         <v>0</v>
       </c>
@@ -2565,7 +2630,7 @@
       <c r="C32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="107">
+      <c r="D32" s="174">
         <f>(10+20)/2</f>
         <v>15</v>
       </c>
@@ -2576,7 +2641,7 @@
         <f>from_geodata!C16</f>
         <v>0</v>
       </c>
-      <c r="G32" s="108">
+      <c r="G32" s="176">
         <f>F32*2*D32</f>
         <v>0</v>
       </c>
@@ -2592,7 +2657,7 @@
       <c r="C33" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="114">
+      <c r="D33" s="177">
         <f>(120+160)/2</f>
         <v>140</v>
       </c>
@@ -2603,7 +2668,7 @@
         <f>from_geodata!C12</f>
         <v>0</v>
       </c>
-      <c r="G33" s="115">
+      <c r="G33" s="184">
         <f>F33*D33</f>
         <v>0</v>
       </c>
@@ -2615,14 +2680,14 @@
       </c>
     </row>
     <row r="34" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="157" t="s">
+      <c r="B34" s="158" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="159"/>
-      <c r="D34" s="160"/>
-      <c r="E34" s="161"/>
-      <c r="F34" s="154"/>
-      <c r="G34" s="111">
+      <c r="C34" s="145"/>
+      <c r="D34" s="146"/>
+      <c r="E34" s="147"/>
+      <c r="F34" s="148"/>
+      <c r="G34" s="182">
         <f>SUM(G29:G33)</f>
         <v>0</v>
       </c>
@@ -2635,25 +2700,25 @@
       <c r="D35" s="69"/>
       <c r="E35" s="69"/>
       <c r="F35" s="70"/>
-      <c r="G35" s="112"/>
+      <c r="G35" s="183"/>
       <c r="H35" s="26"/>
       <c r="I35" s="27"/>
     </row>
     <row r="36" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="158" t="s">
+      <c r="B36" s="160" t="s">
         <v>65</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="107">
+      <c r="D36" s="174">
         <v>0.93</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>105</v>
       </c>
       <c r="F36" s="52"/>
-      <c r="G36" s="108">
+      <c r="G36" s="176">
         <f>F36*D36</f>
         <v>0</v>
       </c>
@@ -2667,7 +2732,7 @@
       <c r="C37" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="114">
+      <c r="D37" s="177">
         <f>AVERAGE(1000, 2000)</f>
         <v>1500</v>
       </c>
@@ -2675,7 +2740,7 @@
         <v>107</v>
       </c>
       <c r="F37" s="66"/>
-      <c r="G37" s="115">
+      <c r="G37" s="184">
         <f>F37*D37</f>
         <v>0</v>
       </c>
@@ -2685,14 +2750,14 @@
       </c>
     </row>
     <row r="38" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="157" t="s">
+      <c r="B38" s="158" t="s">
         <v>69</v>
       </c>
       <c r="C38" s="156"/>
       <c r="D38" s="156"/>
       <c r="E38" s="156"/>
       <c r="F38" s="156"/>
-      <c r="G38" s="111">
+      <c r="G38" s="182">
         <f>SUM(G36:G37)</f>
         <v>0</v>
       </c>
@@ -2705,25 +2770,25 @@
       <c r="D39" s="69"/>
       <c r="E39" s="69"/>
       <c r="F39" s="70"/>
-      <c r="G39" s="112"/>
+      <c r="G39" s="183"/>
       <c r="H39" s="15"/>
       <c r="I39" s="16"/>
     </row>
     <row r="40" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="158" t="s">
+      <c r="B40" s="160" t="s">
         <v>70</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="107">
+      <c r="D40" s="174">
         <v>200</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>106</v>
       </c>
       <c r="F40" s="52"/>
-      <c r="G40" s="108">
+      <c r="G40" s="176">
         <f t="shared" ref="G40:G47" si="1">F40*D40</f>
         <v>0</v>
       </c>
@@ -2737,14 +2802,14 @@
       <c r="C41" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="107">
+      <c r="D41" s="174">
         <v>1500</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>108</v>
       </c>
       <c r="F41" s="52"/>
-      <c r="G41" s="108">
+      <c r="G41" s="176">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2754,18 +2819,18 @@
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="159"/>
+      <c r="B42" s="145"/>
       <c r="C42" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="116">
+      <c r="D42" s="178">
         <v>100</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>107</v>
       </c>
       <c r="F42" s="53"/>
-      <c r="G42" s="117">
+      <c r="G42" s="185">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2777,18 +2842,18 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="159"/>
+      <c r="B43" s="145"/>
       <c r="C43" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D43" s="116">
+      <c r="D43" s="178">
         <v>140</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>107</v>
       </c>
       <c r="F43" s="53"/>
-      <c r="G43" s="117">
+      <c r="G43" s="185">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2798,18 +2863,18 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="159"/>
+      <c r="B44" s="145"/>
       <c r="C44" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D44" s="116">
+      <c r="D44" s="178">
         <v>275</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>107</v>
       </c>
       <c r="F44" s="53"/>
-      <c r="G44" s="117">
+      <c r="G44" s="185">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2819,18 +2884,18 @@
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="159"/>
+      <c r="B45" s="145"/>
       <c r="C45" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="116">
+      <c r="D45" s="178">
         <v>850</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>105</v>
       </c>
       <c r="F45" s="53"/>
-      <c r="G45" s="117">
+      <c r="G45" s="185">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2840,18 +2905,18 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="159"/>
+      <c r="B46" s="145"/>
       <c r="C46" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="116">
+      <c r="D46" s="178">
         <v>1250</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>105</v>
       </c>
       <c r="F46" s="53"/>
-      <c r="G46" s="117">
+      <c r="G46" s="185">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2865,7 +2930,7 @@
       <c r="C47" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="114">
+      <c r="D47" s="177">
         <f>AVERAGE(3.29, 4.21, 5.65, 2.57, 2.77)*0.91^2</f>
         <v>3.0623138000000005</v>
       </c>
@@ -2873,7 +2938,7 @@
         <v>105</v>
       </c>
       <c r="F47" s="66"/>
-      <c r="G47" s="115">
+      <c r="G47" s="184">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2883,14 +2948,14 @@
       </c>
     </row>
     <row r="48" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="157" t="s">
+      <c r="B48" s="158" t="s">
         <v>81</v>
       </c>
       <c r="C48" s="156"/>
       <c r="D48" s="156"/>
       <c r="E48" s="156"/>
       <c r="F48" s="156"/>
-      <c r="G48" s="111">
+      <c r="G48" s="182">
         <f>SUM(G40:G47)</f>
         <v>0</v>
       </c>
@@ -2903,19 +2968,19 @@
       <c r="D49" s="71"/>
       <c r="E49" s="71"/>
       <c r="F49" s="72"/>
-      <c r="G49" s="121"/>
+      <c r="G49" s="187"/>
       <c r="H49" s="37"/>
       <c r="I49" s="38"/>
     </row>
     <row r="50" spans="2:9" s="130" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="155" t="s">
+      <c r="B50" s="157" t="s">
         <v>82</v>
       </c>
       <c r="C50" s="156"/>
       <c r="D50" s="156"/>
       <c r="E50" s="156"/>
       <c r="F50" s="156"/>
-      <c r="G50" s="122">
+      <c r="G50" s="188">
         <f>SUM(G48,G38,G34,G27,G17,G10)</f>
         <v>0</v>
       </c>
@@ -2923,16 +2988,16 @@
       <c r="I50" s="38"/>
     </row>
     <row r="52" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="164" t="s">
+      <c r="B52" s="149" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="159"/>
-      <c r="D52" s="160"/>
-      <c r="E52" s="161"/>
-      <c r="F52" s="154"/>
-      <c r="G52" s="165"/>
-      <c r="H52" s="148"/>
-      <c r="I52" s="150"/>
+      <c r="C52" s="145"/>
+      <c r="D52" s="146"/>
+      <c r="E52" s="147"/>
+      <c r="F52" s="148"/>
+      <c r="G52" s="150"/>
+      <c r="H52" s="151"/>
+      <c r="I52" s="152"/>
     </row>
     <row r="53" spans="2:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="32"/>
@@ -2945,10 +3010,10 @@
       <c r="I53" s="32"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="166" t="s">
+      <c r="B54" s="153" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="159"/>
+      <c r="C54" s="145"/>
       <c r="D54" s="31"/>
       <c r="E54" s="28"/>
       <c r="F54" s="55"/>
@@ -2957,10 +3022,10 @@
       <c r="I54" s="30"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="167" t="s">
+      <c r="B55" s="154" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="159"/>
+      <c r="C55" s="145"/>
       <c r="D55" s="34">
         <v>0.1</v>
       </c>
@@ -2970,7 +3035,7 @@
       <c r="F55" s="135">
         <v>1</v>
       </c>
-      <c r="G55" s="136">
+      <c r="G55" s="189">
         <f>G50*D55</f>
         <v>0</v>
       </c>
@@ -2979,10 +3044,10 @@
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B56" s="167" t="s">
+      <c r="B56" s="154" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="159"/>
+      <c r="C56" s="145"/>
       <c r="D56" s="35">
         <v>0.1</v>
       </c>
@@ -2992,7 +3057,7 @@
       <c r="F56" s="135">
         <v>1</v>
       </c>
-      <c r="G56" s="136">
+      <c r="G56" s="189">
         <f>G50*D56</f>
         <v>0</v>
       </c>
@@ -3001,10 +3066,10 @@
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B57" s="166" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" s="159"/>
+      <c r="B57" s="153" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="145"/>
       <c r="D57" s="36"/>
       <c r="E57" s="28"/>
       <c r="F57" s="55"/>
@@ -3013,8 +3078,8 @@
       <c r="I57" s="30"/>
     </row>
     <row r="58" spans="2:9" s="130" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="168" t="s">
-        <v>119</v>
+      <c r="B58" s="193" t="s">
+        <v>121</v>
       </c>
       <c r="C58" s="156"/>
       <c r="D58" s="143">
@@ -3026,18 +3091,18 @@
       <c r="F58" s="60">
         <v>1</v>
       </c>
-      <c r="G58" s="124">
+      <c r="G58" s="190">
         <f>G50*D58</f>
         <v>0</v>
       </c>
       <c r="H58" s="37"/>
       <c r="I58" s="38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="2:9" s="142" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="168" t="s">
-        <v>120</v>
+      <c r="B59" s="155" t="s">
+        <v>118</v>
       </c>
       <c r="C59" s="156"/>
       <c r="D59" s="58">
@@ -3049,7 +3114,7 @@
       <c r="F59" s="60">
         <v>1</v>
       </c>
-      <c r="G59" s="124">
+      <c r="G59" s="190">
         <f>G50*D59</f>
         <v>0</v>
       </c>
@@ -3057,14 +3122,14 @@
       <c r="I59" s="38"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B61" s="163" t="s">
+      <c r="B61" s="144" t="s">
         <v>88</v>
       </c>
-      <c r="C61" s="159"/>
-      <c r="D61" s="160"/>
-      <c r="E61" s="161"/>
-      <c r="F61" s="154"/>
-      <c r="G61" s="125">
+      <c r="C61" s="145"/>
+      <c r="D61" s="146"/>
+      <c r="E61" s="147"/>
+      <c r="F61" s="148"/>
+      <c r="G61" s="191">
         <f>G58+G56+G55+G50</f>
         <v>0</v>
       </c>
@@ -3073,14 +3138,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="B50:F50"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B12:B16"/>
@@ -3093,12 +3156,14 @@
     <mergeCell ref="B38:F38"/>
     <mergeCell ref="B40:B47"/>
     <mergeCell ref="B48:F48"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:F11 B17:F18 B27:F28 B34:F35 B38:F39 B48:F49">
     <cfRule type="expression" dxfId="9" priority="5">
@@ -3131,8 +3196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3152,16 +3217,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="163" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
     </row>
     <row r="2" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="75" t="s">
@@ -3179,15 +3244,15 @@
         <f>G61</f>
         <v>0</v>
       </c>
-      <c r="H2" s="147" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="149" t="str">
+      <c r="H2" s="164" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="165" t="str">
         <f>IF(NOT(OR(ISBLANK(G2), ISBLANK(G3))),G2/G3,"")</f>
         <v/>
       </c>
       <c r="J2" s="81"/>
-      <c r="K2" s="151" t="s">
+      <c r="K2" s="166" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3199,15 +3264,15 @@
         <v>97</v>
       </c>
       <c r="D3" s="80"/>
-      <c r="E3" s="153" t="s">
-        <v>117</v>
-      </c>
-      <c r="F3" s="154"/>
+      <c r="E3" s="168" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="148"/>
       <c r="G3" s="99"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="150"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="152"/>
       <c r="J3" s="81"/>
-      <c r="K3" s="152"/>
+      <c r="K3" s="167"/>
     </row>
     <row r="4" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="82"/>
@@ -3256,7 +3321,7 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="144" t="s">
+      <c r="B7" s="162" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -3282,7 +3347,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" s="91" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="145"/>
+      <c r="B8" s="159"/>
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
@@ -3307,7 +3372,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="145"/>
+      <c r="B9" s="159"/>
       <c r="C9" s="61" t="s">
         <v>19</v>
       </c>
@@ -3328,13 +3393,13 @@
       </c>
     </row>
     <row r="10" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="158" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="145"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="145"/>
+      <c r="C10" s="159"/>
+      <c r="D10" s="159"/>
+      <c r="E10" s="159"/>
+      <c r="F10" s="159"/>
       <c r="G10" s="111">
         <f>SUM(G7:G9)</f>
         <v>0</v>
@@ -3353,7 +3418,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="2:11" s="91" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="158" t="s">
+      <c r="B12" s="160" t="s">
         <v>109</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -3476,7 +3541,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="157" t="s">
+      <c r="B17" s="158" t="s">
         <v>110</v>
       </c>
       <c r="C17" s="156"/>
@@ -3501,7 +3566,7 @@
       <c r="I18" s="16"/>
     </row>
     <row r="19" spans="2:9" s="90" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="158" t="s">
+      <c r="B19" s="160" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -3525,7 +3590,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="159"/>
+      <c r="B20" s="145"/>
       <c r="C20" s="9" t="s">
         <v>40</v>
       </c>
@@ -3647,7 +3712,7 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="159"/>
+      <c r="B25" s="145"/>
       <c r="C25" s="22" t="s">
         <v>49</v>
       </c>
@@ -3672,7 +3737,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="159"/>
+      <c r="B26" s="145"/>
       <c r="C26" s="67" t="s">
         <v>51</v>
       </c>
@@ -3697,13 +3762,13 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="157" t="s">
+      <c r="B27" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="159"/>
-      <c r="D27" s="160"/>
-      <c r="E27" s="161"/>
-      <c r="F27" s="154"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="146"/>
+      <c r="E27" s="147"/>
+      <c r="F27" s="148"/>
       <c r="G27" s="111">
         <f>SUM(G19:G26)</f>
         <v>0</v>
@@ -3722,7 +3787,7 @@
       <c r="I28" s="27"/>
     </row>
     <row r="29" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="162" t="s">
+      <c r="B29" s="161" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="9" t="s">
@@ -3748,7 +3813,7 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="159"/>
+      <c r="B30" s="145"/>
       <c r="C30" s="9" t="s">
         <v>56</v>
       </c>
@@ -3772,7 +3837,7 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="159"/>
+      <c r="B31" s="145"/>
       <c r="C31" s="9" t="s">
         <v>58</v>
       </c>
@@ -3850,13 +3915,13 @@
       </c>
     </row>
     <row r="34" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="157" t="s">
+      <c r="B34" s="158" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="159"/>
-      <c r="D34" s="160"/>
-      <c r="E34" s="161"/>
-      <c r="F34" s="154"/>
+      <c r="C34" s="145"/>
+      <c r="D34" s="146"/>
+      <c r="E34" s="147"/>
+      <c r="F34" s="148"/>
       <c r="G34" s="111">
         <f>SUM(G29:G33)</f>
         <v>0</v>
@@ -3875,7 +3940,7 @@
       <c r="I35" s="27"/>
     </row>
     <row r="36" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="158" t="s">
+      <c r="B36" s="160" t="s">
         <v>65</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -3921,7 +3986,7 @@
       </c>
     </row>
     <row r="38" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="157" t="s">
+      <c r="B38" s="158" t="s">
         <v>69</v>
       </c>
       <c r="C38" s="156"/>
@@ -3946,7 +4011,7 @@
       <c r="I39" s="16"/>
     </row>
     <row r="40" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="158" t="s">
+      <c r="B40" s="160" t="s">
         <v>70</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -3991,7 +4056,7 @@
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="159"/>
+      <c r="B42" s="145"/>
       <c r="C42" s="9" t="s">
         <v>74</v>
       </c>
@@ -4014,7 +4079,7 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="159"/>
+      <c r="B43" s="145"/>
       <c r="C43" s="9" t="s">
         <v>76</v>
       </c>
@@ -4035,7 +4100,7 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="159"/>
+      <c r="B44" s="145"/>
       <c r="C44" s="9" t="s">
         <v>77</v>
       </c>
@@ -4056,7 +4121,7 @@
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="159"/>
+      <c r="B45" s="145"/>
       <c r="C45" s="9" t="s">
         <v>78</v>
       </c>
@@ -4077,7 +4142,7 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="159"/>
+      <c r="B46" s="145"/>
       <c r="C46" s="9" t="s">
         <v>79</v>
       </c>
@@ -4120,7 +4185,7 @@
       </c>
     </row>
     <row r="48" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="157" t="s">
+      <c r="B48" s="158" t="s">
         <v>81</v>
       </c>
       <c r="C48" s="156"/>
@@ -4145,7 +4210,7 @@
       <c r="I49" s="38"/>
     </row>
     <row r="50" spans="2:9" s="90" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="155" t="s">
+      <c r="B50" s="157" t="s">
         <v>82</v>
       </c>
       <c r="C50" s="156"/>
@@ -4160,16 +4225,16 @@
       <c r="I50" s="38"/>
     </row>
     <row r="52" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="164" t="s">
+      <c r="B52" s="149" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="159"/>
-      <c r="D52" s="160"/>
-      <c r="E52" s="161"/>
-      <c r="F52" s="154"/>
-      <c r="G52" s="165"/>
-      <c r="H52" s="148"/>
-      <c r="I52" s="150"/>
+      <c r="C52" s="145"/>
+      <c r="D52" s="146"/>
+      <c r="E52" s="147"/>
+      <c r="F52" s="148"/>
+      <c r="G52" s="150"/>
+      <c r="H52" s="151"/>
+      <c r="I52" s="152"/>
     </row>
     <row r="53" spans="2:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="32"/>
@@ -4182,10 +4247,10 @@
       <c r="I53" s="32"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="166" t="s">
+      <c r="B54" s="153" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="159"/>
+      <c r="C54" s="145"/>
       <c r="D54" s="31"/>
       <c r="E54" s="28"/>
       <c r="F54" s="55"/>
@@ -4194,10 +4259,10 @@
       <c r="I54" s="30"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="167" t="s">
+      <c r="B55" s="154" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="159"/>
+      <c r="C55" s="145"/>
       <c r="D55" s="34">
         <v>0.1</v>
       </c>
@@ -4216,10 +4281,10 @@
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B56" s="167" t="s">
+      <c r="B56" s="154" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="159"/>
+      <c r="C56" s="145"/>
       <c r="D56" s="35">
         <v>0.1</v>
       </c>
@@ -4238,10 +4303,10 @@
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B57" s="166" t="s">
-        <v>118</v>
-      </c>
-      <c r="C57" s="159"/>
+      <c r="B57" s="153" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="145"/>
       <c r="D57" s="36"/>
       <c r="E57" s="28"/>
       <c r="F57" s="55"/>
@@ -4250,8 +4315,8 @@
       <c r="I57" s="30"/>
     </row>
     <row r="58" spans="2:9" s="90" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="168" t="s">
-        <v>119</v>
+      <c r="B58" s="193" t="s">
+        <v>121</v>
       </c>
       <c r="C58" s="156"/>
       <c r="D58" s="143">
@@ -4269,12 +4334,12 @@
       </c>
       <c r="H58" s="37"/>
       <c r="I58" s="38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="2:9" s="141" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="168" t="s">
-        <v>120</v>
+      <c r="B59" s="155" t="s">
+        <v>118</v>
       </c>
       <c r="C59" s="156"/>
       <c r="D59" s="58">
@@ -4294,13 +4359,13 @@
       <c r="I59" s="38"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B61" s="163" t="s">
+      <c r="B61" s="144" t="s">
         <v>88</v>
       </c>
-      <c r="C61" s="159"/>
-      <c r="D61" s="160"/>
-      <c r="E61" s="161"/>
-      <c r="F61" s="154"/>
+      <c r="C61" s="145"/>
+      <c r="D61" s="146"/>
+      <c r="E61" s="147"/>
+      <c r="F61" s="148"/>
       <c r="G61" s="125">
         <f>G58+G56+G55+G50+G59</f>
         <v>0</v>
@@ -4310,6 +4375,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B59:C59"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="B48:F48"/>
@@ -4326,16 +4401,6 @@
     <mergeCell ref="B29:B33"/>
     <mergeCell ref="B36:B37"/>
     <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B59:C59"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:F11 B17:F18 B27:F28 B34:F35 B38:F39 B48:F49">
     <cfRule type="expression" dxfId="4" priority="5">

</xml_diff>